<commit_message>
Fixed bug last day hydro inflows
</commit_message>
<xml_diff>
--- a/dati_casoStudioItalia/Hydro_inflows_2024.xlsx
+++ b/dati_casoStudioItalia/Hydro_inflows_2024.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\0954659\PycharmProjects\DrinDrin---Mix-energetico\dati_casoStudioItalia\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AEBBE6B-9F4E-4117-BA10-771459660DBB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3D3236C-76A5-4446-B811-52CA490015EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="0" windowWidth="11712" windowHeight="12336" tabRatio="937" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="937" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="pumped_storage_open_inflows" sheetId="1" r:id="rId1"/>
@@ -540,8 +540,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H53"/>
   <sheetViews>
-    <sheetView topLeftCell="A43" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K14" activeCellId="1" sqref="L1:S3 K14"/>
+    <sheetView tabSelected="1" topLeftCell="A43" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C54" sqref="A54:C56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1938,8 +1938,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:H53"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M14" activeCellId="1" sqref="L1:S3 M14"/>
+    <sheetView topLeftCell="A40" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A54" sqref="A54:B54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3337,7 +3337,7 @@
   <dimension ref="A1:H53"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L1" sqref="L1:S3"/>
+      <selection activeCell="B54" sqref="B54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4734,7 +4734,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A2:K28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="J18" sqref="J18"/>
     </sheetView>
   </sheetViews>
@@ -5212,31 +5212,31 @@
         <v>28</v>
       </c>
       <c r="B20" s="5">
-        <f>B10+B13</f>
+        <f t="shared" ref="B20:H20" si="4">B10+B13</f>
         <v>5205.058</v>
       </c>
       <c r="C20" s="5">
-        <f>C10+C13</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="D20" s="5">
-        <f>D10+D13</f>
+        <f t="shared" si="4"/>
         <v>1763</v>
       </c>
       <c r="E20" s="5">
-        <f>E10+E13</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="F20" s="5">
-        <f>F10+F13</f>
+        <f t="shared" si="4"/>
         <v>240</v>
       </c>
       <c r="G20" s="5">
-        <f>G10+G13</f>
+        <f t="shared" si="4"/>
         <v>580</v>
       </c>
       <c r="H20" s="5">
-        <f>H10+H13</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="J20" s="9"/>
@@ -5253,18 +5253,18 @@
         <v>0</v>
       </c>
       <c r="D21" s="5">
-        <f t="shared" ref="C21:H21" si="4">D19/D20</f>
+        <f t="shared" ref="D21:G21" si="5">D19/D20</f>
         <v>53.879750425411231</v>
       </c>
       <c r="E21" s="5">
         <v>0</v>
       </c>
       <c r="F21" s="5">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="G21" s="5">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="H21" s="5">
@@ -5275,7 +5275,7 @@
         <v>37.106811479832331</v>
       </c>
       <c r="J21" s="9">
-        <f t="shared" ref="J19:J23" si="5">1/I21</f>
+        <f t="shared" ref="J21:J23" si="6">1/I21</f>
         <v>2.6949230077165296E-2</v>
       </c>
       <c r="K21" t="s">
@@ -5287,31 +5287,31 @@
         <v>27</v>
       </c>
       <c r="B22" s="5">
-        <f>-B11</f>
+        <f t="shared" ref="B22:H22" si="7">-B11</f>
         <v>1751</v>
       </c>
       <c r="C22" s="5">
-        <f>-C11</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="D22" s="5">
-        <f>-D11</f>
+        <f t="shared" si="7"/>
         <v>333</v>
       </c>
       <c r="E22" s="5">
-        <f>-E11</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="F22" s="5">
-        <f>-F11</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="G22" s="5">
-        <f>-G11</f>
+        <f t="shared" si="7"/>
         <v>58</v>
       </c>
       <c r="H22" s="5">
-        <f>-H11</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="J22" s="9"/>
@@ -5325,7 +5325,7 @@
         <v>110.79383209594518</v>
       </c>
       <c r="D23">
-        <f t="shared" ref="C23:H23" si="6">D19/D22</f>
+        <f t="shared" ref="D23" si="8">D19/D22</f>
         <v>285.25525525525524</v>
       </c>
       <c r="I23">
@@ -5333,7 +5333,7 @@
         <v>134.91596638655463</v>
       </c>
       <c r="J23" s="9">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>7.4120211772033626E-3</v>
       </c>
       <c r="K23" t="s">
@@ -5349,27 +5349,27 @@
         <v>194000</v>
       </c>
       <c r="C25" s="5">
-        <f t="shared" ref="C25:H25" si="7">C12*1000</f>
+        <f t="shared" ref="C25:H25" si="9">C12*1000</f>
         <v>0</v>
       </c>
       <c r="D25" s="5">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>94990</v>
       </c>
       <c r="E25" s="5">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="F25" s="5">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="G25" s="5">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="H25" s="5">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
@@ -5382,27 +5382,27 @@
         <v>5205.058</v>
       </c>
       <c r="C26" s="5">
-        <f t="shared" ref="C26:H26" si="8">C10+C13</f>
+        <f t="shared" ref="C26:H26" si="10">C10+C13</f>
         <v>0</v>
       </c>
       <c r="D26" s="5">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>1763</v>
       </c>
       <c r="E26" s="5">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="F26" s="5">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>240</v>
       </c>
       <c r="G26" s="5">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>580</v>
       </c>
       <c r="H26" s="5">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
     </row>
@@ -5415,7 +5415,7 @@
         <v>2.6830195876288661E-2</v>
       </c>
       <c r="D27">
-        <f t="shared" ref="D27" si="9">D26/D25</f>
+        <f t="shared" ref="D27" si="11">D26/D25</f>
         <v>1.8559848405095274E-2</v>
       </c>
     </row>
@@ -5428,27 +5428,27 @@
         <v>1751</v>
       </c>
       <c r="C28" s="5">
-        <f t="shared" ref="C28:H28" si="10">-C11</f>
+        <f t="shared" ref="C28:H28" si="12">-C11</f>
         <v>0</v>
       </c>
       <c r="D28" s="5">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>333</v>
       </c>
       <c r="E28" s="5">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="F28" s="5">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="G28" s="5">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>58</v>
       </c>
       <c r="H28" s="5">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
     </row>

</xml_diff>